<commit_message>
Sugestões sobre os requisitos
</commit_message>
<xml_diff>
--- a/Fabrica.de.Festas.xlsx
+++ b/Fabrica.de.Festas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Educação\Christus\2016.1\APIS\Projeto Final\fabrica-de-festas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Descrição</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Sistema Fábrica de Festas</t>
+  </si>
+  <si>
+    <t>O termo "Manter" para o caso de Estoque não é adequado, pois o CRUD para esse tipo de entidade é bem diferenciado. Assim, ao invés de cadastrar, existe o "Adicionar" ou "Dar Entrada" no estoque. Ao invés de remover, existe o "Dar Baixa" no estoque. Portanto, devem ser casos de uso diferentes.</t>
+  </si>
+  <si>
+    <t>A parte de pagamentos está fora do sistema?</t>
+  </si>
+  <si>
+    <t>Quando vocês descrevem "Relatório de Orçamentos", a idéia que passa é de uma coisa fixa, um relatório. Já o nome "manter orçamentos" dá uma idéia de CRUD. Isso merece uma reflexão e melhoria.</t>
   </si>
 </sst>
 </file>
@@ -159,15 +168,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,29 +474,29 @@
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -498,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -512,7 +524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -526,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -540,7 +552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -554,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -568,7 +580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -582,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -596,7 +608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -610,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -624,9 +636,38 @@
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B17:H17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>